<commit_message>
feat: Added prediction algorithm
</commit_message>
<xml_diff>
--- a/diets/utils/meals_v2.xlsx
+++ b/diets/utils/meals_v2.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\diet_and_control\diets\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067B663E-8A1F-43F6-A561-D464999771CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1266F46B-836C-4087-9E83-D6E87C789FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3735" windowWidth="38700" windowHeight="15345" firstSheet="1" activeTab="1" xr2:uid="{A373EF7D-856A-473D-8B16-30DE7D3A582A}"/>
+    <workbookView xWindow="0" yWindow="4890" windowWidth="38700" windowHeight="15345" xr2:uid="{A373EF7D-856A-473D-8B16-30DE7D3A582A}"/>
   </bookViews>
   <sheets>
-    <sheet name="DatosPacientes" sheetId="1" r:id="rId1"/>
+    <sheet name="patients_data" sheetId="1" r:id="rId1"/>
     <sheet name="menus" sheetId="2" r:id="rId2"/>
     <sheet name="meals" sheetId="6" r:id="rId3"/>
   </sheets>
@@ -62,15 +62,9 @@
     <t>ENFERMEDAD</t>
   </si>
   <si>
-    <t xml:space="preserve">Plan </t>
-  </si>
-  <si>
     <t>Femenino</t>
   </si>
   <si>
-    <t xml:space="preserve">Obesidad </t>
-  </si>
-  <si>
     <t>Id_Plan pk</t>
   </si>
   <si>
@@ -363,6 +357,12 @@
   </si>
   <si>
     <t>https://img.freepik.com/foto-gratis/deliciosa-comida-vietnamita-que-incluye-pho-ga-fideos-rollitos-primavera-mesa-blanca_181624-34062.jpg?size=626&amp;ext=jpg&amp;ga=GA1.2.1683082823.1629158434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN </t>
+  </si>
+  <si>
+    <t>OBESIDAD</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -519,6 +518,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665A5EB3-648C-4B0F-A60C-2DC2A5FC50B6}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,8 +871,8 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
+      <c r="I1" s="16" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -878,7 +880,7 @@
         <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>31.2</v>
@@ -896,35 +898,10 @@
         <v>466</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="I2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I7">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDD8C32-35AE-4502-A17D-01163AEC8328}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -954,34 +931,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1225,40 +1202,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>73</v>
+      <c r="L1" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1266,10 +1243,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2">
         <v>27.6</v>
@@ -1296,7 +1273,7 @@
         <v>24.1</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1304,10 +1281,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>69.300000000000011</v>
@@ -1334,7 +1311,7 @@
         <v>48.7</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1342,10 +1319,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>12.5</v>
@@ -1372,7 +1349,7 @@
         <v>3.4</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1380,10 +1357,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>15.3</v>
@@ -1410,7 +1387,7 @@
         <v>13.8</v>
       </c>
       <c r="L5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1418,10 +1395,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <v>148.70000000000002</v>
@@ -1448,7 +1425,7 @@
         <v>92.4</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1456,10 +1433,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>120.60000000000001</v>
@@ -1486,7 +1463,7 @@
         <v>88.9</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1494,10 +1471,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>30.599999999999998</v>
@@ -1524,7 +1501,7 @@
         <v>21.4</v>
       </c>
       <c r="L8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1532,10 +1509,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>10.799999999999999</v>
@@ -1562,7 +1539,7 @@
         <v>10.7</v>
       </c>
       <c r="L9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1570,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>15.6</v>
@@ -1600,7 +1577,7 @@
         <v>0.5</v>
       </c>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1608,10 +1585,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11">
         <v>73.8</v>
@@ -1638,7 +1615,7 @@
         <v>46.6</v>
       </c>
       <c r="L11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1646,10 +1623,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>28.700000000000003</v>
@@ -1676,7 +1653,7 @@
         <v>14.4</v>
       </c>
       <c r="L12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1684,10 +1661,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>11.9</v>
@@ -1714,7 +1691,7 @@
         <v>9.4</v>
       </c>
       <c r="L13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1722,10 +1699,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>15.4</v>
@@ -1752,7 +1729,7 @@
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1760,10 +1737,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>38.799999999999997</v>
@@ -1790,7 +1767,7 @@
         <v>20.100000000000001</v>
       </c>
       <c r="L15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1798,10 +1775,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>99.6</v>
@@ -1828,7 +1805,7 @@
         <v>59.1</v>
       </c>
       <c r="L16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1836,10 +1813,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <v>27.2</v>
@@ -1866,7 +1843,7 @@
         <v>26.5</v>
       </c>
       <c r="L17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1874,10 +1851,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>20.099999999999998</v>
@@ -1894,17 +1871,17 @@
       <c r="H18">
         <v>69.599999999999994</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="12">
         <v>1.5</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="12">
         <v>1.2</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="12">
         <v>17.399999999999999</v>
       </c>
       <c r="L18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1912,10 +1889,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>129.39999999999998</v>
@@ -1942,7 +1919,7 @@
         <v>76.8</v>
       </c>
       <c r="L19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1950,42 +1927,42 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="14">
+        <v>31</v>
+      </c>
+      <c r="D20" s="13">
         <f>SUM(I20:K20)</f>
         <v>19.298000000000002</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <f>SUM(F20:H20)</f>
         <v>86.177000000000007</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="13">
         <f>I20*4</f>
         <v>13.3</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <f>J20*9</f>
         <v>16.173000000000002</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <f>K20*4</f>
         <v>56.704000000000001</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <v>3.3250000000000002</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <v>1.7970000000000002</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="13">
         <v>14.176</v>
       </c>
       <c r="L20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1993,10 +1970,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2023,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2031,10 +2008,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22">
         <f t="shared" ref="D22" si="0">SUM(I22:K22)</f>
@@ -2066,7 +2043,7 @@
         <v>17.8</v>
       </c>
       <c r="L22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2074,10 +2051,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23">
         <f>SUM(I23:K23)</f>
@@ -2109,7 +2086,7 @@
         <v>28.84</v>
       </c>
       <c r="L23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2117,10 +2094,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <f t="shared" ref="D24:D36" si="5">SUM(I24:K24)</f>
@@ -2142,17 +2119,17 @@
         <f t="shared" si="4"/>
         <v>258</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="14">
         <v>24.400000000000002</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="14">
         <v>8.85</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="14">
         <v>64.5</v>
       </c>
       <c r="L24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2160,42 +2137,42 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="14">
+        <v>34</v>
+      </c>
+      <c r="D25" s="13">
         <f t="shared" si="5"/>
         <v>22.564999999999998</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="13">
         <f t="shared" si="6"/>
         <v>167.98500000000001</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="13">
         <f t="shared" si="7"/>
         <v>3.2039999999999997</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <f t="shared" si="8"/>
         <v>139.905</v>
       </c>
-      <c r="H25" s="14">
+      <c r="H25" s="13">
         <f t="shared" si="4"/>
         <v>24.875999999999998</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="15">
         <v>0.80099999999999993</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="15">
         <v>15.545</v>
       </c>
-      <c r="K25" s="16">
+      <c r="K25" s="15">
         <v>6.2189999999999994</v>
       </c>
       <c r="L25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2203,28 +2180,28 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="14">
+        <v>38</v>
+      </c>
+      <c r="D26" s="13">
         <f t="shared" si="5"/>
         <v>110.4</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="13">
         <f t="shared" si="6"/>
         <v>460.6</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="13">
         <f t="shared" si="7"/>
         <v>108.4</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <f t="shared" si="8"/>
         <v>34.199999999999996</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="13">
         <f t="shared" si="4"/>
         <v>318</v>
       </c>
@@ -2238,7 +2215,7 @@
         <v>79.5</v>
       </c>
       <c r="L26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2246,28 +2223,28 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="14">
+        <v>34</v>
+      </c>
+      <c r="D27" s="13">
         <f t="shared" si="5"/>
         <v>21.799999999999997</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="13">
         <f t="shared" si="6"/>
         <v>164.7</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="13">
         <f t="shared" si="7"/>
         <v>11.6</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <f t="shared" si="8"/>
         <v>139.5</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="13">
         <f t="shared" si="4"/>
         <v>13.6</v>
       </c>
@@ -2281,7 +2258,7 @@
         <v>3.4</v>
       </c>
       <c r="L27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2289,25 +2266,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="14">
+        <v>62</v>
+      </c>
+      <c r="D28" s="13">
         <f t="shared" si="5"/>
         <v>22.700000000000003</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="13">
         <f t="shared" si="6"/>
         <v>143.30000000000001</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="13">
         <f t="shared" si="7"/>
         <v>7.2</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <f t="shared" si="8"/>
         <v>94.5</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="13">
         <f t="shared" si="4"/>
         <v>41.6</v>
       </c>
@@ -2321,7 +2298,7 @@
         <v>10.4</v>
       </c>
       <c r="L28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2329,42 +2306,42 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="14">
+        <v>45</v>
+      </c>
+      <c r="D29" s="13">
         <f t="shared" si="5"/>
         <v>90.054000000000002</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="13">
         <f t="shared" si="6"/>
         <v>448.15600000000001</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="13">
         <f t="shared" si="7"/>
         <v>93.980000000000018</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <f t="shared" si="8"/>
         <v>158.292</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="13">
         <f t="shared" si="4"/>
         <v>195.88399999999999</v>
       </c>
-      <c r="I29" s="16">
+      <c r="I29" s="15">
         <v>23.495000000000005</v>
       </c>
-      <c r="J29" s="16">
+      <c r="J29" s="15">
         <v>17.588000000000001</v>
       </c>
-      <c r="K29" s="16">
+      <c r="K29" s="15">
         <v>48.970999999999997</v>
       </c>
       <c r="L29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2372,42 +2349,42 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="14">
+        <v>38</v>
+      </c>
+      <c r="D30" s="13">
         <f t="shared" si="5"/>
         <v>138.90399999999997</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="13">
         <f t="shared" si="6"/>
         <v>654.80099999999993</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="13">
         <f t="shared" si="7"/>
         <v>132.90399999999997</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <f t="shared" si="8"/>
         <v>178.53299999999999</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="13">
         <f t="shared" si="4"/>
         <v>343.36399999999992</v>
       </c>
-      <c r="I30" s="16">
+      <c r="I30" s="15">
         <v>33.225999999999992</v>
       </c>
-      <c r="J30" s="16">
+      <c r="J30" s="15">
         <v>19.837</v>
       </c>
-      <c r="K30" s="16">
+      <c r="K30" s="15">
         <v>85.84099999999998</v>
       </c>
       <c r="L30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2415,28 +2392,28 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="14">
+        <v>36</v>
+      </c>
+      <c r="D31" s="13">
         <f t="shared" si="5"/>
         <v>10.4</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="13">
         <f t="shared" si="6"/>
         <v>45.6</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="13">
         <f t="shared" si="7"/>
         <v>2.8</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <f t="shared" si="8"/>
         <v>7.2</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="13">
         <f t="shared" si="4"/>
         <v>35.6</v>
       </c>
@@ -2450,7 +2427,7 @@
         <v>8.9</v>
       </c>
       <c r="L31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2458,42 +2435,42 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="14">
+        <v>38</v>
+      </c>
+      <c r="D32" s="13">
         <f t="shared" si="5"/>
         <v>91</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="13">
         <f t="shared" si="6"/>
         <v>381</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="13">
         <f t="shared" si="7"/>
         <v>102</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <f t="shared" si="8"/>
         <v>30.599999999999998</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="13">
         <f t="shared" si="4"/>
         <v>248.4</v>
       </c>
-      <c r="I32" s="15">
+      <c r="I32" s="14">
         <v>25.5</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="14">
         <v>3.4</v>
       </c>
-      <c r="K32" s="15">
+      <c r="K32" s="14">
         <v>62.1</v>
       </c>
       <c r="L32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2501,28 +2478,28 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="14">
+        <v>31</v>
+      </c>
+      <c r="D33" s="13">
         <f t="shared" si="5"/>
         <v>53.4</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="13">
         <f t="shared" si="6"/>
         <v>266.10000000000002</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="13">
         <f t="shared" si="7"/>
         <v>42.4</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <f t="shared" si="8"/>
         <v>94.5</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="13">
         <f t="shared" si="4"/>
         <v>129.19999999999999</v>
       </c>
@@ -2536,7 +2513,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="L33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2544,28 +2521,28 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="14">
+        <v>31</v>
+      </c>
+      <c r="D34" s="13">
         <f t="shared" si="5"/>
         <v>35.299999999999997</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="13">
         <f t="shared" si="6"/>
         <v>191.7</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="13">
         <f t="shared" si="7"/>
         <v>34</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <f t="shared" si="8"/>
         <v>90.899999999999991</v>
       </c>
-      <c r="H34" s="14">
+      <c r="H34" s="13">
         <f t="shared" si="4"/>
         <v>66.8</v>
       </c>
@@ -2579,7 +2556,7 @@
         <v>16.7</v>
       </c>
       <c r="L34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2587,28 +2564,28 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="14">
+        <v>36</v>
+      </c>
+      <c r="D35" s="13">
         <f t="shared" si="5"/>
         <v>27.4</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="13">
         <f t="shared" si="6"/>
         <v>111.6</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="13">
         <f t="shared" si="7"/>
         <v>7.2</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <f t="shared" si="8"/>
         <v>3.6</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H35" s="13">
         <f t="shared" si="4"/>
         <v>100.8</v>
       </c>
@@ -2622,7 +2599,7 @@
         <v>25.2</v>
       </c>
       <c r="L35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2630,42 +2607,42 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="14">
+        <v>36</v>
+      </c>
+      <c r="D36" s="13">
         <f t="shared" si="5"/>
         <v>13.899999999999999</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="13">
         <f t="shared" si="6"/>
         <v>93.6</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="13">
         <f t="shared" si="7"/>
         <v>13.2</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <f t="shared" si="8"/>
         <v>68.399999999999991</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="13">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="I36" s="15">
+      <c r="I36" s="14">
         <v>3.3</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="14">
         <v>7.6</v>
       </c>
-      <c r="K36" s="15">
+      <c r="K36" s="14">
         <v>3</v>
       </c>
       <c r="L36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>